<commit_message>
Build error resolved (#357)
</commit_message>
<xml_diff>
--- a/samples/virtualan-sv-all/src/test/resources/virtualan_bdd_testcase_run_manager_1.xlsx
+++ b/samples/virtualan-sv-all/src/test/resources/virtualan_bdd_testcase_run_manager_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\July13\virtualan\samples\virtualan-spring-boot\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\virtualan\samples\virtualan-sv-all\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE656CD3-2AE4-42FE-8E48-B7A2A1301EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6C51D0-7BD8-44A3-B03A-BF2456131744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API-Testing" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>id;name;category.id;category.name</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>api</t>
   </si>
 </sst>
 </file>
@@ -575,198 +581,216 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K1001"/>
+  <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="176.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.71875" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" customWidth="1"/>
-    <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="8" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="176.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="8" max="9" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="332.7">
+    <row r="3" spans="1:12" ht="357.75">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="270">
+    <row r="4" spans="1:12" ht="285">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="295.8">
+    <row r="5" spans="1:12" ht="332.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="280.8">
+    <row r="6" spans="1:12" ht="285.75">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>201</v>
       </c>
     </row>
@@ -1751,21 +1775,21 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="G2:H3">
+  <conditionalFormatting sqref="H2:I3">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(G2))&gt;0</formula>
+      <formula>LEN(TRIM(H2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:H5">
+  <conditionalFormatting sqref="H5:I5">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(G5))&gt;0</formula>
+      <formula>LEN(TRIM(H5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{89F7A190-55D8-4F5C-A883-BD0AA5D7BDDE}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{4159AF51-DCA6-4B63-A814-01596194D032}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{89F7A190-55D8-4F5C-A883-BD0AA5D7BDDE}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{4159AF51-DCA6-4B63-A814-01596194D032}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>

</xml_diff>